<commit_message>
add version 0.2 of pascal to C (part2)
</commit_message>
<xml_diff>
--- a/docs/interim-report/文法目标代码对应关系.xlsx
+++ b/docs/interim-report/文法目标代码对应关系.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20358"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC24C615-8136-4AE6-96BC-27EEDD991967}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2671B4-4E83-48EA-A23F-215F0C6F2ECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>文法</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -740,212 +740,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">variable_list -&gt; variable_list, { </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>} variable | variable</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>下标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">compound_statement -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">begin </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{ 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">if (!compound_statement.is_subprogram_body) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-} statement_list </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> end</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{ 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    if </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(!compound_statement.is_subprogram_body) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-}</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1392,8 +1187,601 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">statement -&gt; variable </t>
+    <t>表达式列表，用于函数传参以及输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注：复合语句作为子程序的body时，C语言需要先在函数体内部声明常量和变量，再执行语句。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">procedure_call -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>void id()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> } | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">id( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">void id( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">} expression_list {
+    int count = 0;    
+    for (auto exp : expression_list) {
+        if (count != 0) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ;
+        if (isPointer(id.args[count++])) {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+            if (isPointer(exp)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>exp.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">;
+            else </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;exp.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+        }
+        else {
+            if (isPointer(exp)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>*exp.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">;
+            else </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>exp.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 
+        }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    }
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">term -&gt; term </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mulop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>factor {term.content = term.content + mulop + factor.content} 
+| factor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {term.content = factor.content}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">simple_expression -&gt; simple_expression </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>addop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> term {simple_expression.content = simple_expression.content + addop + term.content} 
+| term</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {simple_expression.content = term.content}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">expression -&gt; simple_expression </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>relop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> simple_expression {expression.content = simple_expression.content + relop + simple_expression.content}
+| simple_expression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {expression.content = simple_expression.content}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">id_varpart -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression_list {
+    int count = 0;
+    for (auto exp : expression_list) 
+        id_varpart.content += "[" + str(exp.content - id[count++].base) + "]"
+}</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>| e</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">variable -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id_varpart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {variable.content = id + id_varpart.content}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expression_list -&gt; expression_list, expression {
+    expression_list = expression_list;
+    expression_list.push_back(expression);
+} 
+| expression {expression_list.push_back(expression)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>variable_list -&gt; variable_list, variable {
+    variable_list = variable_list;
+    variable_list.push_back(variable);
+} 
+| variable {variable_list.push_back(variable)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">statement -&gt; variable {
+    if (isPointer(variable)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*variable.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
+    else </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variable.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+} </t>
     </r>
     <r>
       <rPr>
@@ -1439,9 +1827,78 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> } expression
+      <t xml:space="preserve"> } expression { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> }
 | procedure_call 
-| compound_statement
+| { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> } compound_statement { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">}
 | </t>
     </r>
     <r>
@@ -1488,7 +1945,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">} expression { </t>
+      <t>} expression {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> expression.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -1719,7 +2199,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">} expression </t>
+      <t>} expression {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> expression.content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> } </t>
     </r>
     <r>
       <rPr>
@@ -1754,18 +2257,41 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> ; id != </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>} expression {</t>
+      <t xml:space="preserve"> ; id &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">} expression { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">expression.content </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>} {</t>
     </r>
     <r>
       <rPr>
@@ -2032,7 +2558,7 @@
     string s, t;
     for (auto exp : expression_list) {
         s += map[exp.type];
-        t += ", " + exp.text;
+        t += ", " + exp.content;
     }
    </t>
     </r>
@@ -2110,198 +2636,93 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>表达式列表，用于函数传参以及输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">variable -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{
-    if (variable.output) {
-        if (varialbe.in_call &amp;&amp; isPointer(function_args[variable.pos])) {
-            // 该变量在传参列表中，且对应位置为引用调用
-            if (isPointer(variable)) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">;    
-            else </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">;
+    <r>
+      <t xml:space="preserve">factor -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">num </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{ factor.content = num}
+| variable {factor.content = variable.content}
+| </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression_list</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{
+    factor.content = id + "("
+    int count = 0;    
+    for (auto exp : expression_list) {
+        if (count != 0) factor.content += "," ;
+        if (isPointer(id.args[count++])) {
+            if (isPointer(exp)) factor.content += exp.content;
+            else factor.content += "&amp;" + exp.content;
         }
-        else if (isPointer(variable)) {
-           </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (*id)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>;
-        }
-        else</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>;
-    }
-}
-id_varpart</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">id_varpart -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">expression_list {
-    if (id_varpart.output) {
-        int count = 0;
-        for (auto exp : expression_list) {
-            </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[exp.text - id[count++].base ]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+        else {
+            if (isPointer(exp)) factor.content += "*" + exp.content;
+            else factor.content += exp.content; 
         }
     }
+    factor.content += ")"
 }</t>
     </r>
     <r>
@@ -2314,172 +2735,136 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>| e</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注：复合语句作为子程序的body时，C语言需要先在函数体内部声明常量和变量，再执行语句。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">procedure_call -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>void id()</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> } | </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">id( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">void id( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">} expression_list {
-    int count = 0;    
-    for (auto exp : expression_list) {
-         if (isPointer(id.args[count++])) 
-    }
-}
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{factor.content = "(" + expression.content + ")"}</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> factor {factor.content = "!" + factor.content}
+| </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">uminus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>factor {factor.content = "-" + factor.content}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2488,7 +2873,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2519,6 +2904,25 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2835,8 +3239,8 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2851,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -2862,7 +3266,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -2881,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="154" x14ac:dyDescent="0.3">
@@ -2889,18 +3293,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="70" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="56" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
+      <c r="B6" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -2911,54 +3315,54 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="336" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="406" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="70" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="196" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="112" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="84" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="98" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="242" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -2972,52 +3376,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="70" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="56" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="56" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="84" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="294" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3"/>
     </row>

</xml_diff>